<commit_message>
planilha de roteamento de IPs
</commit_message>
<xml_diff>
--- a/Exercícios/exLucas22-10-19/PROJETO DE ROTEAMENTO E VLAN.xlsx
+++ b/Exercícios/exLucas22-10-19/PROJETO DE ROTEAMENTO E VLAN.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\exLucas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\36952457860\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A40B6B-E5E7-4ED0-A571-FEBD10AAEE69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{9AF423C3-3506-41BD-ADFF-60D39E9A4B99}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="92">
   <si>
     <t>REDE 1</t>
   </si>
@@ -256,12 +255,57 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>IP rede 172.16.1.0 - Masc Rede 255.255.255.128</t>
+  </si>
+  <si>
+    <t>IP rede 172.16.0.0 - Masc Rede 255.255.255.0</t>
+  </si>
+  <si>
+    <t>IP rede 172.16.1.128 - Masc Rede 255.255.255.240</t>
+  </si>
+  <si>
+    <t>172.16.2.0/26</t>
+  </si>
+  <si>
+    <t>172.16.2.0 - masc 255.255.255.192</t>
+  </si>
+  <si>
+    <t>172.16.2.64/26</t>
+  </si>
+  <si>
+    <t>172.16.2.64 - masc 255.255.255.192</t>
+  </si>
+  <si>
+    <t>192.16.2.74</t>
+  </si>
+  <si>
+    <t>172.16.2.128/27</t>
+  </si>
+  <si>
+    <t>172.16.2.128 - masc 255.255.255.224</t>
+  </si>
+  <si>
+    <t>172.16.2.160/27</t>
+  </si>
+  <si>
+    <t>172.16.2.160 - masc 255.255.255.224</t>
+  </si>
+  <si>
+    <t>192.16.2.75</t>
+  </si>
+  <si>
+    <t>192.16.2.76</t>
+  </si>
+  <si>
+    <t>192.16.2.77</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -325,7 +369,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +415,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -486,6 +536,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,11 +851,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB9F082-6E60-4088-BDCC-D3969D453C29}">
-  <dimension ref="A1:I38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -811,11 +863,11 @@
     <col min="1" max="1" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="41.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.7109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
@@ -904,22 +956,24 @@
       <c r="C6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="25" t="s">
         <v>67</v>
       </c>
       <c r="E6" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="24">
         <v>10</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="I6" s="25" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
@@ -937,16 +991,16 @@
       <c r="E7" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="27">
         <v>20</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="2"/>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
@@ -991,16 +1045,18 @@
       <c r="E9" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="24">
         <v>10</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="25" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -1015,16 +1071,16 @@
       <c r="D10" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="27">
         <v>20</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="I10" s="28"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
@@ -1063,16 +1119,18 @@
       <c r="D12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="24">
         <v>10</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="I12" s="2"/>
+      <c r="I12" s="25" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
@@ -1087,16 +1145,16 @@
       <c r="D13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="27">
         <v>20</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="I13" s="28"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -1126,16 +1184,18 @@
       <c r="A15" s="12"/>
       <c r="B15" s="13"/>
       <c r="C15" s="11"/>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="24">
         <v>10</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="I15" s="2"/>
+      <c r="I15" s="25" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1143,18 +1203,18 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="27">
         <v>20</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="28"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>3</v>
       </c>
@@ -1178,7 +1238,7 @@
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
         <v>10</v>
       </c>
@@ -1188,7 +1248,9 @@
       <c r="C18" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="F18" s="3" t="s">
         <v>36</v>
       </c>
@@ -1200,7 +1262,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
         <v>20</v>
       </c>
@@ -1210,7 +1272,9 @@
       <c r="C19" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="28" t="s">
+        <v>78</v>
+      </c>
       <c r="F19" s="3" t="s">
         <v>37</v>
       </c>
@@ -1222,7 +1286,7 @@
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
         <v>100</v>
       </c>
@@ -1232,7 +1296,9 @@
       <c r="C20" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="30" t="s">
+        <v>79</v>
+      </c>
       <c r="F20" s="3" t="s">
         <v>39</v>
       </c>
@@ -1244,7 +1310,7 @@
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>99</v>
       </c>
@@ -1264,7 +1330,7 @@
       </c>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F22" s="3" t="s">
         <v>40</v>
       </c>
@@ -1276,13 +1342,13 @@
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D23"/>
       <c r="F23" s="12"/>
       <c r="G23" s="13"/>
       <c r="H23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C24" s="20"/>
       <c r="D24" s="19"/>
       <c r="F24" s="5" t="s">
@@ -1291,7 +1357,7 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D25" s="19"/>
       <c r="F25" s="4" t="s">
         <v>3</v>
@@ -1303,27 +1369,38 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D26"/>
-      <c r="F26" s="3">
+      <c r="F26" s="24">
         <v>10</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="I26" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D27"/>
-      <c r="F27" s="3">
+      <c r="F27" s="27">
         <v>20</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H27" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="I27" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="K27" s="20"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D28"/>
       <c r="F28" s="3">
         <v>30</v>
@@ -1331,9 +1408,14 @@
       <c r="G28" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D29"/>
       <c r="F29" s="3">
         <v>100</v>
@@ -1341,9 +1423,14 @@
       <c r="G29" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D30"/>
       <c r="F30" s="3">
         <v>99</v>
@@ -1353,10 +1440,10 @@
       </c>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>42</v>
       </c>
@@ -1364,7 +1451,7 @@
       <c r="C32" s="10"/>
       <c r="D32" s="20"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>1</v>
       </c>
@@ -1372,20 +1459,21 @@
         <v>43</v>
       </c>
       <c r="C33" s="11"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H33" s="31"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="13"/>
       <c r="C34" s="11"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>2</v>
       </c>
@@ -1397,7 +1485,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
@@ -1409,7 +1497,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>32</v>
       </c>

</xml_diff>